<commit_message>
Sd phase de l essai creation conceptmap (#54)
* creation de la concepmap valueset et codesystem

creation de la concepmap valueset et codesystem

* precision conceptmap

utilisation de wider et ajout jarde-early

* correction CS

* correction casesensitvie CS et modif conceptmap

* typo

* précision définition title 36a3931e18a3c24a6ee446fa14e8d4ea8858b9ff
</commit_message>
<xml_diff>
--- a/ig/main/CodeSystem-eclaire-study-phase-code-system.xlsx
+++ b/ig/main/CodeSystem-eclaire-study-phase-code-system.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-30T13:32:08+00:00</t>
+    <t>2023-09-01T08:48:57+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -87,6 +87,9 @@
     <t>Case Sensitive</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>Value Set (all codes)</t>
   </si>
   <si>
@@ -130,6 +133,9 @@
   </si>
   <si>
     <t>Phase III and phase IV (Integrated)</t>
+  </si>
+  <si>
+    <t>Trials that are a combination of phases III and IV.</t>
   </si>
 </sst>
 </file>
@@ -375,52 +381,54 @@
       <c r="A14" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" t="s" s="2">
+        <v>24</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -438,29 +446,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="D2" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="D2" t="s" s="2">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Sd typo phase 3 et 4 (#66)
* correction typo

* typos essei dans description 205768818ac4c5c3015a115647f5550c27e59ccd
</commit_message>
<xml_diff>
--- a/ig/main/CodeSystem-eclaire-study-phase-code-system.xlsx
+++ b/ig/main/CodeSystem-eclaire-study-phase-code-system.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-09-15T14:08:50+00:00</t>
+    <t>2023-09-15T14:15:22+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -132,10 +132,10 @@
     <t>phase-3-phase-4</t>
   </si>
   <si>
-    <t>Phase III and phase IV (Integrated)</t>
-  </si>
-  <si>
-    <t>Trials that are a combination of phases III and IV.</t>
+    <t>Phase 3 and phase 4</t>
+  </si>
+  <si>
+    <t>Trials that are a combination of phases 3 and 4.</t>
   </si>
 </sst>
 </file>

</xml_diff>